<commit_message>
udpated data dictionary for the sankey app including cancer outcomes
</commit_message>
<xml_diff>
--- a/eval_sankey/sankey_data_dictionary.xlsx
+++ b/eval_sankey/sankey_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/eval_sankey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc_new/eval_sankey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE18738A-8E01-44EB-929C-9FE8B8B85246}"/>
+  <xr:revisionPtr revIDLastSave="377" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAFA6172-E041-42C8-9410-AE7D7FE50A1C}"/>
   <bookViews>
-    <workbookView xWindow="26385" yWindow="9360" windowWidth="24240" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6390" yWindow="11835" windowWidth="21915" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="171">
   <si>
     <t>field</t>
   </si>
@@ -200,9 +200,6 @@
     <t>3+ scans</t>
   </si>
   <si>
-    <t>Loss to follow up</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -428,9 +425,6 @@
     <t>The number of unique participants in the invites table who have two valid scan records (dated and outcomed as being performed) in the LDCT table.</t>
   </si>
   <si>
-    <t>The number of participants for whom we currently have no follow-up information about. We will update this group when we have cancer diagnosis and staging information.</t>
-  </si>
-  <si>
     <t>The number of unique participants in the invites table who have no follow-up information recorded in either the LHC, Measurements or LDCT tables.</t>
   </si>
   <si>
@@ -441,6 +435,120 @@
   </si>
   <si>
     <t>The number of participants whose LHC contacts / attempted contacts are recorded as face-to-face.</t>
+  </si>
+  <si>
+    <t>Not scanned</t>
+  </si>
+  <si>
+    <t>The number of participants who were not scanned as part of the TLHC programme</t>
+  </si>
+  <si>
+    <t>cancer_outcome</t>
+  </si>
+  <si>
+    <t>NCRAS consolidated cancer outcomes</t>
+  </si>
+  <si>
+    <t>The number of participants who had at least one low-dose CT scan and do not appear in the NCRAS dataset with a diagnosis of lung cancer.</t>
+  </si>
+  <si>
+    <t>The number of unique participants in the LDCT table with at least one valid scan records (dated and outcomed as being performed) but do not appear in the NCRAS dataset with a lung cancer diagnosis.</t>
+  </si>
+  <si>
+    <t>TLHC: lung cancer</t>
+  </si>
+  <si>
+    <t>LDCT AND NCRAS consolidated cancer outcomes</t>
+  </si>
+  <si>
+    <t>LHC AND LDCT AND NCRAS consolidated cancer outcomes</t>
+  </si>
+  <si>
+    <t>The number of participants with a low-dose CT scan or were assessed as high risk at LHC and a lung cancer diagnosed within 147 days of their TLHC contact.</t>
+  </si>
+  <si>
+    <t>The number of participants who had either a) a low-dose CT scan or b) a LHC at which they were assessed as being high risk and eligible for a scan, and also have a lung cancer diagnosed within 147 days of their TLHC contact  in the NCRAS dataset.</t>
+  </si>
+  <si>
+    <t>No lung cancer</t>
+  </si>
+  <si>
+    <t>The number of participants who were not scanned as part of the TLHC programme and do not have a lung cancer diagnosis.</t>
+  </si>
+  <si>
+    <t>The number of unique participants in the invites table who have no follow-up information recorded in either the LHC, Measurements or LDCT tables and are not found with a lung cancer diagnosis in the NCRAS dataset.</t>
+  </si>
+  <si>
+    <t>Counterfactual: lung cancer</t>
+  </si>
+  <si>
+    <t>Invites AND LHC AND Measurements AND LDCT AND NCRAS consolidated cancer outcomes</t>
+  </si>
+  <si>
+    <t>The number of people who have a lung cancer diagnosis which is not associated with TLHC activity because they did not take up the offer of a LHC, or attended LHC but were assessed as low risk, or even had a scan but the diagnosis was made over 147 days following their scan.</t>
+  </si>
+  <si>
+    <t>The number of unique particiapnts in the invites table who have a lung cancer diagnosis in the NCRAS dataset but which is not associated with TLHC activity either because the participant didn't receive a scan (were invited but didn't take up the offer, attended LHC but were assessed as low risk) or did receive a scan but the diagnosis was made over 147 days afterwards.</t>
+  </si>
+  <si>
+    <t>cancer_stage</t>
+  </si>
+  <si>
+    <t>TLHC: S 1-2</t>
+  </si>
+  <si>
+    <t>The number of people with a TLHC-associated lung cancer, with a stage of either 1 or 2.</t>
+  </si>
+  <si>
+    <t>TLHC: S 3-4</t>
+  </si>
+  <si>
+    <t>The number of people with a TLHC-associated lung cancer, with a stage of either 3 or 4.</t>
+  </si>
+  <si>
+    <t>TLHC: S ?</t>
+  </si>
+  <si>
+    <t>The number of people with a TLHC-associated lung cancer which is not staged.</t>
+  </si>
+  <si>
+    <t>C: S 1-2</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 147 days of a TLHC scan or LHC at which they were assessed as high risk and with a Tumour-Node-Metastasis (TNM) staging of either 1 or 2.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 147 days of a TLHC scan or LHC at which they were assessed as high risk and with a Tumour-Node-Metastasis (TNM) staging of either 3 or 4.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis with a Tumour-Node-Metastasis (TNM) staging of either 1 or 2 and where the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 147 days following scan.</t>
+  </si>
+  <si>
+    <t>C: S 3-4</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis with a Tumour-Node-Metastasis (TNM) staging of either 3 or 4 and where the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 147 days following scan.</t>
+  </si>
+  <si>
+    <t>C: S ?</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 147 days of a TLHC scan or LHC at which they were assessed as high risk and staging information is not provided because there is insufficient information or the cancer is unstageable.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis is without staging information because there is insufficient information or the cancer is unstageable and the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 147 days following scan.</t>
+  </si>
+  <si>
+    <t>The number of people with a lung cancer staged at 3 or 4 and is not associated with TLHC activity (counterfactual).</t>
+  </si>
+  <si>
+    <t>The number of people with a lung cancer which is not staged and is not associated with TLHC activity (counterfactual).</t>
+  </si>
+  <si>
+    <t>The number of people with a lung cancer staged at 1 or 2 and is not associated with TLHC activity (counterfactual).</t>
+  </si>
+  <si>
+    <t>Scanned: No lung cancer</t>
   </si>
 </sst>
 </file>
@@ -521,8 +629,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}" name="Table1" displayName="Table1" ref="A1:E38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E38" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}" name="Table1" displayName="Table1" ref="A1:E48" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E48" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{885DF6EA-C1AE-4DCA-8379-8003415977E3}" name="field" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2611AB96-2DE8-4599-AAE8-7CC66A03B70D}" name="value" dataDxfId="3"/>
@@ -797,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -841,10 +949,10 @@
         <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -858,10 +966,10 @@
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -875,10 +983,10 @@
         <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -892,10 +1000,10 @@
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -909,10 +1017,10 @@
         <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -926,10 +1034,10 @@
         <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -943,10 +1051,10 @@
         <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -960,10 +1068,10 @@
         <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -977,10 +1085,10 @@
         <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -994,10 +1102,10 @@
         <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1011,10 +1119,10 @@
         <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1028,10 +1136,10 @@
         <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1045,10 +1153,10 @@
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1062,10 +1170,10 @@
         <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1079,10 +1187,10 @@
         <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1096,10 +1204,10 @@
         <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1113,10 +1221,10 @@
         <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1130,10 +1238,10 @@
         <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1147,10 +1255,10 @@
         <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1164,10 +1272,10 @@
         <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1181,10 +1289,10 @@
         <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1198,10 +1306,10 @@
         <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1215,10 +1323,10 @@
         <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1232,10 +1340,10 @@
         <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1249,10 +1357,10 @@
         <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1266,10 +1374,10 @@
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1280,13 +1388,13 @@
         <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1300,10 +1408,10 @@
         <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1317,10 +1425,10 @@
         <v>42</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1331,13 +1439,13 @@
         <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1351,10 +1459,10 @@
         <v>42</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1368,10 +1476,10 @@
         <v>42</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1382,13 +1490,13 @@
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1399,13 +1507,13 @@
         <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1416,13 +1524,13 @@
         <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1433,30 +1541,200 @@
         <v>53</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds data dictionary for the sankey app
</commit_message>
<xml_diff>
--- a/eval_sankey/sankey_data_dictionary.xlsx
+++ b/eval_sankey/sankey_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc_new/eval_sankey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAFA6172-E041-42C8-9410-AE7D7FE50A1C}"/>
+  <xr:revisionPtr revIDLastSave="395" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12C46EB2-0039-4B93-AFDA-73C47EC2A335}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="11835" windowWidth="21915" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6150" yWindow="5280" windowWidth="48240" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="174">
   <si>
     <t>field</t>
   </si>
@@ -452,9 +452,6 @@
     <t>The number of participants who had at least one low-dose CT scan and do not appear in the NCRAS dataset with a diagnosis of lung cancer.</t>
   </si>
   <si>
-    <t>The number of unique participants in the LDCT table with at least one valid scan records (dated and outcomed as being performed) but do not appear in the NCRAS dataset with a lung cancer diagnosis.</t>
-  </si>
-  <si>
     <t>TLHC: lung cancer</t>
   </si>
   <si>
@@ -464,12 +461,6 @@
     <t>LHC AND LDCT AND NCRAS consolidated cancer outcomes</t>
   </si>
   <si>
-    <t>The number of participants with a low-dose CT scan or were assessed as high risk at LHC and a lung cancer diagnosed within 147 days of their TLHC contact.</t>
-  </si>
-  <si>
-    <t>The number of participants who had either a) a low-dose CT scan or b) a LHC at which they were assessed as being high risk and eligible for a scan, and also have a lung cancer diagnosed within 147 days of their TLHC contact  in the NCRAS dataset.</t>
-  </si>
-  <si>
     <t>No lung cancer</t>
   </si>
   <si>
@@ -485,12 +476,6 @@
     <t>Invites AND LHC AND Measurements AND LDCT AND NCRAS consolidated cancer outcomes</t>
   </si>
   <si>
-    <t>The number of people who have a lung cancer diagnosis which is not associated with TLHC activity because they did not take up the offer of a LHC, or attended LHC but were assessed as low risk, or even had a scan but the diagnosis was made over 147 days following their scan.</t>
-  </si>
-  <si>
-    <t>The number of unique particiapnts in the invites table who have a lung cancer diagnosis in the NCRAS dataset but which is not associated with TLHC activity either because the participant didn't receive a scan (were invited but didn't take up the offer, attended LHC but were assessed as low risk) or did receive a scan but the diagnosis was made over 147 days afterwards.</t>
-  </si>
-  <si>
     <t>cancer_stage</t>
   </si>
   <si>
@@ -515,30 +500,12 @@
     <t>C: S 1-2</t>
   </si>
   <si>
-    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 147 days of a TLHC scan or LHC at which they were assessed as high risk and with a Tumour-Node-Metastasis (TNM) staging of either 1 or 2.</t>
-  </si>
-  <si>
-    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 147 days of a TLHC scan or LHC at which they were assessed as high risk and with a Tumour-Node-Metastasis (TNM) staging of either 3 or 4.</t>
-  </si>
-  <si>
-    <t>The number of unique participants with a lung cancer diagnosis with a Tumour-Node-Metastasis (TNM) staging of either 1 or 2 and where the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 147 days following scan.</t>
-  </si>
-  <si>
     <t>C: S 3-4</t>
   </si>
   <si>
-    <t>The number of unique participants with a lung cancer diagnosis with a Tumour-Node-Metastasis (TNM) staging of either 3 or 4 and where the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 147 days following scan.</t>
-  </si>
-  <si>
     <t>C: S ?</t>
   </si>
   <si>
-    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 147 days of a TLHC scan or LHC at which they were assessed as high risk and staging information is not provided because there is insufficient information or the cancer is unstageable.</t>
-  </si>
-  <si>
-    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis is without staging information because there is insufficient information or the cancer is unstageable and the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 147 days following scan.</t>
-  </si>
-  <si>
     <t>The number of people with a lung cancer staged at 3 or 4 and is not associated with TLHC activity (counterfactual).</t>
   </si>
   <si>
@@ -549,6 +516,48 @@
   </si>
   <si>
     <t>Scanned: No lung cancer</t>
+  </si>
+  <si>
+    <t>The number of participants with a low-dose CT scan or were assessed as high risk at LHC and a lung cancer diagnosed within 185 days of their TLHC contact.</t>
+  </si>
+  <si>
+    <t>The number of participants who had either a) a low-dose CT scan or b) a LHC at which they were assessed as being high risk and eligible for a scan, and also have a lung cancer diagnosed within 185 days of their TLHC contact  in the NCRAS dataset.</t>
+  </si>
+  <si>
+    <t>The number of people who have a lung cancer diagnosis which is not associated with TLHC activity because they did not take up the offer of a LHC, or attended LHC but were assessed as low risk, or even had a scan but the diagnosis was made over 185 days following their scan.</t>
+  </si>
+  <si>
+    <t>The number of unique particiapnts in the invites table who have a lung cancer diagnosis in the NCRAS dataset but which is not associated with TLHC activity either because the participant didn't receive a scan (were invited but didn't take up the offer, attended LHC but were assessed as low risk) or did receive a scan but the diagnosis was made over 185 days afterwards.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 185 days of a TLHC scan or LHC at which they were assessed as high risk and with a Tumour-Node-Metastasis (TNM) staging of either 1 or 2.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 185 days of a TLHC scan or LHC at which they were assessed as high risk and with a Tumour-Node-Metastasis (TNM) staging of either 3 or 4.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis was made within 185 days of a TLHC scan or LHC at which they were assessed as high risk and staging information is not provided because there is insufficient information or the cancer is unstageable.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis with a Tumour-Node-Metastasis (TNM) staging of either 1 or 2 and where the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 185 days following scan.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis with a Tumour-Node-Metastasis (TNM) staging of either 3 or 4 and where the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 185 days following scan.</t>
+  </si>
+  <si>
+    <t>The number of unique participants with a lung cancer diagnosis where the diagnosis is without staging information because there is insufficient information or the cancer is unstageable and the diagnosis is not associated with TLHC activity because the participant did not undergo a scan or the diagnosis was made over 185 days following scan.</t>
+  </si>
+  <si>
+    <t>Scanned: Awaiting results</t>
+  </si>
+  <si>
+    <t>The number of participants who had at least one low-dose CT scan and do not appear in the NCRAS dataset with a diagnosis of lung cancer and where their scan took place after the period covered by NCRAS data.</t>
+  </si>
+  <si>
+    <t>The number of unique participants in the LDCT table with at least one valid scan record (dated and outcomed as being performed) but do not appear in the NCRAS dataset with a lung cancer diagnosis.</t>
+  </si>
+  <si>
+    <t>The number of unique participants in the LDCT table with at least one valid scan record (dated and outcomed as being performed) but do not appear in the NCRAS dataset with a lung cancer diagnosis and where the scan took place after 27th Feb 2023 (185 days before the end of the NCRAS cancer diagnosis data) meaning we are unsure of the result of the scan.</t>
   </si>
 </sst>
 </file>
@@ -584,9 +593,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,8 +641,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}" name="Table1" displayName="Table1" ref="A1:E48" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E48" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E49" xr:uid="{E115BC42-6375-4EE8-ABB1-F1DCC0986E27}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{885DF6EA-C1AE-4DCA-8379-8003415977E3}" name="field" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2611AB96-2DE8-4599-AAE8-7CC66A03B70D}" name="value" dataDxfId="3"/>
@@ -905,11 +917,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -918,7 +928,10 @@
     <col min="3" max="3" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="71.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="20" width="9.140625" style="1"/>
+    <col min="21" max="21" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1465,7 +1478,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -1482,7 +1495,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -1499,7 +1512,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
@@ -1516,7 +1529,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
@@ -1533,7 +1546,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1550,7 +1563,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -1567,174 +1580,193 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>166</v>
+    </row>
+    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>